<commit_message>
Fixed anonmization issue in the descriptive data.
</commit_message>
<xml_diff>
--- a/data/StatisticalData/participants_descriptive.xlsx
+++ b/data/StatisticalData/participants_descriptive.xlsx
@@ -8,34 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\code\Momentum\PedestrianData\data\StatisticalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD836DBA-2335-4B61-A04E-E13578238276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42770C0-9E61-40F2-9474-7B88E2CD58E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B16C5A67-FA4D-4197-AB5A-C9A44F25FDD9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$J$121</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="71">
   <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>VP Group</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age in years</t>
+  </si>
+  <si>
+    <t>weight in kg</t>
+  </si>
+  <si>
+    <t>height in cm</t>
+  </si>
+  <si>
+    <t>glasses/lenses</t>
+  </si>
+  <si>
+    <t>active driving experience in years</t>
+  </si>
+  <si>
+    <t>accidents experienced as a pedestrian</t>
+  </si>
+  <si>
+    <t>prior experience with VR</t>
+  </si>
+  <si>
     <t>72.7</t>
   </si>
   <si>
@@ -205,36 +224,6 @@
   </si>
   <si>
     <t>53.2</t>
-  </si>
-  <si>
-    <t>VPN</t>
-  </si>
-  <si>
-    <t>VP Group</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>age in years</t>
-  </si>
-  <si>
-    <t>weight in kg</t>
-  </si>
-  <si>
-    <t>height in cm</t>
-  </si>
-  <si>
-    <t>glasses/lenses</t>
-  </si>
-  <si>
-    <t>active driving experience in years</t>
-  </si>
-  <si>
-    <t>accidents experienced as a pedestrian</t>
-  </si>
-  <si>
-    <t>prior experience with VR</t>
   </si>
   <si>
     <t>male</t>
@@ -617,57 +606,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5F97F4-ADC7-4AF7-A03C-E39FF1C348D0}">
-  <dimension ref="A1:J122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="21.453125" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -681,7 +670,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F2">
         <v>187</v>
@@ -699,7 +688,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -731,7 +720,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -745,7 +734,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>186</v>
@@ -754,7 +743,7 @@
         <v>70</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -763,7 +752,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -795,7 +784,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -809,7 +798,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F6">
         <v>171</v>
@@ -827,7 +816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -841,7 +830,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>178</v>
@@ -859,7 +848,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -873,7 +862,7 @@
         <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F8">
         <v>164</v>
@@ -891,7 +880,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -905,7 +894,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>183</v>
@@ -923,7 +912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -937,7 +926,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F10">
         <v>165</v>
@@ -955,7 +944,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -969,7 +958,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F11">
         <v>166</v>
@@ -987,7 +976,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1001,7 +990,7 @@
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F12">
         <v>177</v>
@@ -1019,7 +1008,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1033,10 +1022,10 @@
         <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
         <v>70</v>
@@ -1051,7 +1040,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1065,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>179</v>
@@ -1083,63 +1072,63 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>172</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16">
         <v>44</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15">
+      <c r="E16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16">
         <v>163</v>
       </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15">
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16">
         <v>26</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>188</v>
-      </c>
-      <c r="G16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
       <c r="I16">
         <v>0</v>
       </c>
@@ -1147,12 +1136,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>67</v>
@@ -1161,25 +1150,25 @@
         <v>22</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F17">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="G17" t="s">
         <v>69</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1193,7 +1182,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>180</v>
@@ -1211,7 +1200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1225,16 +1214,16 @@
         <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
         <v>69</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1243,7 +1232,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1257,7 +1246,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F20">
         <v>170</v>
@@ -1275,7 +1264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1289,7 +1278,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F21">
         <v>173</v>
@@ -1307,7 +1296,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1321,7 +1310,7 @@
         <v>21</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F22">
         <v>160</v>
@@ -1339,7 +1328,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1356,7 +1345,7 @@
         <v>43</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
         <v>69</v>
@@ -1371,7 +1360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1385,7 +1374,7 @@
         <v>26</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F24">
         <v>187</v>
@@ -1403,7 +1392,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1417,10 +1406,10 @@
         <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
         <v>69</v>
@@ -1435,7 +1424,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1449,7 +1438,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F26">
         <v>176</v>
@@ -1467,7 +1456,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1481,7 +1470,7 @@
         <v>22</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F27">
         <v>168</v>
@@ -1499,7 +1488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1513,7 +1502,7 @@
         <v>35</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F28">
         <v>171</v>
@@ -1531,7 +1520,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1554,7 +1543,7 @@
         <v>69</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1563,7 +1552,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1577,7 +1566,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F30">
         <v>181</v>
@@ -1595,7 +1584,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1609,7 +1598,7 @@
         <v>31</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F31">
         <v>189</v>
@@ -1627,7 +1616,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1641,7 +1630,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F32">
         <v>173</v>
@@ -1659,7 +1648,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1673,7 +1662,7 @@
         <v>33</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F33">
         <v>187</v>
@@ -1691,7 +1680,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1705,7 +1694,7 @@
         <v>22</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F34">
         <v>173</v>
@@ -1723,7 +1712,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1737,313 +1726,313 @@
         <v>24</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36">
         <v>25</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36">
+      <c r="E36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36">
+        <v>183</v>
+      </c>
+      <c r="G36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36">
+        <v>8</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37">
+        <v>23</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37">
+        <v>167</v>
+      </c>
+      <c r="G37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38">
+        <v>25</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38">
+        <v>176</v>
+      </c>
+      <c r="G38" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39">
+        <v>175</v>
+      </c>
+      <c r="G39" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39">
+        <v>14</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40">
+        <v>21</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40">
+        <v>160</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41">
+        <v>25</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41">
+        <v>180</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42">
+        <v>29</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <v>174</v>
+      </c>
+      <c r="G42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42">
+        <v>12</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43">
+        <v>27</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43">
+        <v>177</v>
+      </c>
+      <c r="G43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44">
         <v>20</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E44" s="2">
         <v>85</v>
       </c>
-      <c r="F36">
+      <c r="F44">
         <v>187</v>
       </c>
-      <c r="G36" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36">
+      <c r="G44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44">
         <v>3</v>
       </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37">
-        <v>25</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37">
-        <v>183</v>
-      </c>
-      <c r="G37" t="s">
-        <v>70</v>
-      </c>
-      <c r="H37">
-        <v>8</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38">
-        <v>23</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38">
-        <v>167</v>
-      </c>
-      <c r="G38" t="s">
-        <v>69</v>
-      </c>
-      <c r="H38">
-        <v>6</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39">
-        <v>25</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39">
-        <v>176</v>
-      </c>
-      <c r="G39" t="s">
-        <v>69</v>
-      </c>
-      <c r="H39">
-        <v>5</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40">
-        <v>32</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40">
-        <v>175</v>
-      </c>
-      <c r="G40" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40">
-        <v>14</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41">
-        <v>21</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>160</v>
-      </c>
-      <c r="G41" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41">
-        <v>3</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42">
-        <v>25</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42">
-        <v>180</v>
-      </c>
-      <c r="G42" t="s">
-        <v>69</v>
-      </c>
-      <c r="H42">
-        <v>7</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43">
-        <v>29</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>174</v>
-      </c>
-      <c r="G43" t="s">
-        <v>69</v>
-      </c>
-      <c r="H43">
-        <v>12</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44">
-        <v>27</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F44">
-        <v>177</v>
-      </c>
-      <c r="G44" t="s">
-        <v>69</v>
-      </c>
-      <c r="H44">
-        <v>8</v>
-      </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2066,7 +2055,7 @@
         <v>69</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -2075,7 +2064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2107,7 +2096,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2121,7 +2110,7 @@
         <v>24</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F47">
         <v>169</v>
@@ -2139,7 +2128,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2153,7 +2142,7 @@
         <v>22</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F48">
         <v>166</v>
@@ -2171,7 +2160,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2203,7 +2192,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2235,7 +2224,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2249,10 +2238,10 @@
         <v>27</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="G51" t="s">
         <v>69</v>
@@ -2267,7 +2256,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2299,7 +2288,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2313,7 +2302,7 @@
         <v>24</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F53">
         <v>180</v>
@@ -2331,7 +2320,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2345,10 +2334,10 @@
         <v>20</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G54" t="s">
         <v>69</v>
@@ -2363,7 +2352,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2377,7 +2366,7 @@
         <v>26</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F55">
         <v>173</v>
@@ -2395,7 +2384,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2409,7 +2398,7 @@
         <v>23</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F56">
         <v>165</v>
@@ -2427,7 +2416,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2441,7 +2430,7 @@
         <v>20</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F57">
         <v>184</v>
@@ -2459,7 +2448,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2491,7 +2480,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2505,7 +2494,7 @@
         <v>26</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F59">
         <v>165</v>
@@ -2523,7 +2512,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2537,7 +2526,7 @@
         <v>24</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F60">
         <v>178</v>
@@ -2555,7 +2544,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2569,7 +2558,7 @@
         <v>26</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F61">
         <v>190</v>
@@ -2587,510 +2576,309 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
     </row>
-    <row r="63" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
     </row>
-    <row r="66" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
     </row>
-    <row r="67" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
     </row>
-    <row r="74" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
     </row>
-    <row r="81" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
     </row>
-    <row r="82" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
     </row>
-    <row r="83" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
     </row>
-    <row r="84" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
     </row>
-    <row r="85" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
     </row>
-    <row r="86" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
     </row>
-    <row r="87" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
     </row>
-    <row r="88" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
     </row>
-    <row r="89" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
     </row>
-    <row r="90" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
     </row>
-    <row r="91" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
     </row>
-    <row r="98" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
     </row>
-    <row r="102" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
     </row>
-    <row r="103" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
     </row>
-    <row r="104" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
     </row>
-    <row r="108" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
     </row>
-    <row r="110" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
     </row>
-    <row r="111" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
     </row>
-    <row r="112" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
     </row>
-    <row r="113" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
     </row>
-    <row r="114" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
     </row>
-    <row r="115" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
     </row>
-    <row r="116" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
     </row>
-    <row r="117" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
     </row>
-    <row r="118" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
     </row>
-    <row r="119" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
     </row>
-    <row r="120" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
     </row>
-    <row r="121" spans="8:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H121" s="7"/>
-      <c r="I121" s="7"/>
-      <c r="J121" s="7"/>
-    </row>
-    <row r="122" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H122" s="5"/>
+    <row r="121" spans="8:10" x14ac:dyDescent="0.35">
+      <c r="H121" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J61">
-    <sortCondition ref="A2:A61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J121">
+    <sortCondition ref="A2:A121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010049E367C10E62FE45BB1DD6A736049119" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2f1f1ba97dfbbcb328bfa32b0bbb9d30">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c5af0214-3345-47f9-8f6c-5499bfcfc256" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a5a3e807fa1f3bdfa6a478f829a2662" ns2:_="">
-    <xsd:import namespace="c5af0214-3345-47f9-8f6c-5499bfcfc256"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c5af0214-3345-47f9-8f6c-5499bfcfc256" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A00F98-E2CC-45EB-B843-9FC03D16ED00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F078BB6-EE9C-4BFB-9DEA-5A0A97D9E34D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ACB5334-172A-4436-AE38-AA0CAF2061D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c5af0214-3345-47f9-8f6c-5499bfcfc256"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>